<commit_message>
CIERRE DEL 29 OCT 21
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 10  OCTUBRE 2021/BALANCE  HERRADURA  OCTUBRE   2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 10  OCTUBRE 2021/BALANCE  HERRADURA  OCTUBRE   2021.xlsx
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="200">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -786,16 +786,25 @@
     <t>SALCHICHA</t>
   </si>
   <si>
-    <t># 6153</t>
-  </si>
-  <si>
-    <t>#  6154</t>
-  </si>
-  <si>
     <t>TOCINO-RETAZO-MAIZ-QUESO-JAMON</t>
   </si>
   <si>
     <t>NOMINA # 42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUESO  </t>
+  </si>
+  <si>
+    <t>JAMON-SALCHICHA-QUESO-LONGANIZA</t>
+  </si>
+  <si>
+    <t># 6661</t>
+  </si>
+  <si>
+    <t>#  6662</t>
+  </si>
+  <si>
+    <t>PAPA-CECINA-TOCINO-ADOBO-QUESO</t>
   </si>
 </sst>
 </file>
@@ -2363,6 +2372,57 @@
     </xf>
     <xf numFmtId="44" fontId="3" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="41" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2418,57 +2478,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4084,23 +4093,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="244"/>
-      <c r="C1" s="253" t="s">
+      <c r="B1" s="225"/>
+      <c r="C1" s="234" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="254"/>
-      <c r="E1" s="254"/>
-      <c r="F1" s="254"/>
-      <c r="G1" s="254"/>
-      <c r="H1" s="254"/>
-      <c r="I1" s="254"/>
-      <c r="J1" s="254"/>
-      <c r="K1" s="254"/>
-      <c r="L1" s="254"/>
-      <c r="M1" s="254"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="235"/>
+      <c r="K1" s="235"/>
+      <c r="L1" s="235"/>
+      <c r="M1" s="235"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="245"/>
+      <c r="B2" s="226"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -4110,17 +4119,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="246" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="247"/>
+      <c r="B3" s="227" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="228"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="248" t="s">
+      <c r="H3" s="229" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="248"/>
+      <c r="I3" s="229"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -4136,14 +4145,14 @@
       <c r="D4" s="16">
         <v>44410</v>
       </c>
-      <c r="E4" s="249" t="s">
+      <c r="E4" s="230" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="250"/>
-      <c r="H4" s="251" t="s">
+      <c r="F4" s="231"/>
+      <c r="H4" s="232" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="252"/>
+      <c r="I4" s="233"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -4153,10 +4162,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="238" t="s">
+      <c r="P4" s="219" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="239"/>
+      <c r="Q4" s="220"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -5651,11 +5660,11 @@
       <c r="L39" s="69">
         <v>454.62</v>
       </c>
-      <c r="M39" s="240">
+      <c r="M39" s="221">
         <f>SUM(M5:M38)</f>
         <v>1393675.5</v>
       </c>
-      <c r="N39" s="242">
+      <c r="N39" s="223">
         <f>SUM(N5:N38)</f>
         <v>28399.97</v>
       </c>
@@ -5687,8 +5696,8 @@
       <c r="L40" s="69">
         <v>1195.67</v>
       </c>
-      <c r="M40" s="241"/>
-      <c r="N40" s="243"/>
+      <c r="M40" s="222"/>
+      <c r="N40" s="224"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -5921,29 +5930,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="228" t="s">
+      <c r="H52" s="245" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="229"/>
+      <c r="I52" s="246"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="230">
+      <c r="K52" s="247">
         <f>I50+L50</f>
         <v>80916.84</v>
       </c>
-      <c r="L52" s="231"/>
-      <c r="M52" s="219">
+      <c r="L52" s="248"/>
+      <c r="M52" s="236">
         <f>N39+M39</f>
         <v>1422075.47</v>
       </c>
-      <c r="N52" s="220"/>
+      <c r="N52" s="237"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="232" t="s">
+      <c r="D53" s="249" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="232"/>
+      <c r="E53" s="249"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1396181.44</v>
@@ -5954,22 +5963,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="233" t="s">
+      <c r="D54" s="250" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="233"/>
+      <c r="E54" s="250"/>
       <c r="F54" s="102">
         <v>-1523111</v>
       </c>
-      <c r="I54" s="234" t="s">
+      <c r="I54" s="251" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="235"/>
-      <c r="K54" s="236">
+      <c r="J54" s="252"/>
+      <c r="K54" s="253">
         <f>F56+F57+F58</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L54" s="237"/>
+      <c r="L54" s="254"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -6000,10 +6009,10 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="221">
-        <v>0</v>
-      </c>
-      <c r="L56" s="222"/>
+      <c r="K56" s="238">
+        <v>0</v>
+      </c>
+      <c r="L56" s="239"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -6020,22 +6029,22 @@
       <c r="C58" s="120">
         <v>44444</v>
       </c>
-      <c r="D58" s="223" t="s">
+      <c r="D58" s="240" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="224"/>
+      <c r="E58" s="241"/>
       <c r="F58" s="121">
         <v>136234.76999999999</v>
       </c>
-      <c r="I58" s="225" t="s">
+      <c r="I58" s="242" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="226"/>
-      <c r="K58" s="227">
+      <c r="J58" s="243"/>
+      <c r="K58" s="244">
         <f>K54+K56</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L58" s="227"/>
+      <c r="L58" s="244"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -6179,15 +6188,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="C1:M1"/>
     <mergeCell ref="M52:N52"/>
     <mergeCell ref="K56:L56"/>
     <mergeCell ref="D58:E58"/>
@@ -6199,6 +6199,15 @@
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7912,23 +7921,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="244"/>
-      <c r="C1" s="253" t="s">
+      <c r="B1" s="225"/>
+      <c r="C1" s="234" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="254"/>
-      <c r="E1" s="254"/>
-      <c r="F1" s="254"/>
-      <c r="G1" s="254"/>
-      <c r="H1" s="254"/>
-      <c r="I1" s="254"/>
-      <c r="J1" s="254"/>
-      <c r="K1" s="254"/>
-      <c r="L1" s="254"/>
-      <c r="M1" s="254"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="235"/>
+      <c r="K1" s="235"/>
+      <c r="L1" s="235"/>
+      <c r="M1" s="235"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="245"/>
+      <c r="B2" s="226"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -7938,17 +7947,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="246" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="247"/>
+      <c r="B3" s="227" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="228"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="248" t="s">
+      <c r="H3" s="229" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="248"/>
+      <c r="I3" s="229"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -7964,14 +7973,14 @@
       <c r="D4" s="16">
         <v>44444</v>
       </c>
-      <c r="E4" s="249" t="s">
+      <c r="E4" s="230" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="250"/>
-      <c r="H4" s="251" t="s">
+      <c r="F4" s="231"/>
+      <c r="H4" s="232" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="252"/>
+      <c r="I4" s="233"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -7981,10 +7990,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="238" t="s">
+      <c r="P4" s="219" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="239"/>
+      <c r="Q4" s="220"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -9474,11 +9483,11 @@
       <c r="J39" s="67"/>
       <c r="K39" s="82"/>
       <c r="L39" s="69"/>
-      <c r="M39" s="240">
+      <c r="M39" s="221">
         <f>SUM(M5:M38)</f>
         <v>1464441</v>
       </c>
-      <c r="N39" s="242">
+      <c r="N39" s="223">
         <f>SUM(N5:N38)</f>
         <v>53494</v>
       </c>
@@ -9504,8 +9513,8 @@
       <c r="J40" s="67"/>
       <c r="K40" s="71"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="241"/>
-      <c r="N40" s="243"/>
+      <c r="M40" s="222"/>
+      <c r="N40" s="224"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -9720,29 +9729,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="228" t="s">
+      <c r="H52" s="245" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="229"/>
+      <c r="I52" s="246"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="230">
+      <c r="K52" s="247">
         <f>I50+L50</f>
         <v>69642.26999999999</v>
       </c>
-      <c r="L52" s="231"/>
-      <c r="M52" s="219">
+      <c r="L52" s="248"/>
+      <c r="M52" s="236">
         <f>N39+M39</f>
         <v>1517935</v>
       </c>
-      <c r="N52" s="220"/>
+      <c r="N52" s="237"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="232" t="s">
+      <c r="D53" s="249" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="232"/>
+      <c r="E53" s="249"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1505921.23</v>
@@ -9753,22 +9762,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="233" t="s">
+      <c r="D54" s="250" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="233"/>
+      <c r="E54" s="250"/>
       <c r="F54" s="102">
         <v>-1424333.95</v>
       </c>
-      <c r="I54" s="234" t="s">
+      <c r="I54" s="251" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="235"/>
-      <c r="K54" s="236">
+      <c r="J54" s="252"/>
+      <c r="K54" s="253">
         <f>F56+F57+F58</f>
         <v>222140.17000000004</v>
       </c>
-      <c r="L54" s="237"/>
+      <c r="L54" s="254"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -9799,11 +9808,11 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="221">
+      <c r="K56" s="238">
         <f>-C4</f>
         <v>-136234.76999999999</v>
       </c>
-      <c r="L56" s="222"/>
+      <c r="L56" s="239"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -9820,22 +9829,22 @@
       <c r="C58" s="120">
         <v>44472</v>
       </c>
-      <c r="D58" s="223" t="s">
+      <c r="D58" s="240" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="224"/>
+      <c r="E58" s="241"/>
       <c r="F58" s="121">
         <v>134848.89000000001</v>
       </c>
-      <c r="I58" s="225" t="s">
+      <c r="I58" s="242" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="226"/>
-      <c r="K58" s="227">
+      <c r="J58" s="243"/>
+      <c r="K58" s="244">
         <f>K54+K56</f>
         <v>85905.400000000052</v>
       </c>
-      <c r="L58" s="227"/>
+      <c r="L58" s="244"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -9979,12 +9988,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -9999,6 +10002,12 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -11595,8 +11604,8 @@
   </sheetPr>
   <dimension ref="A1:S80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11618,23 +11627,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="244"/>
-      <c r="C1" s="253" t="s">
+      <c r="B1" s="225"/>
+      <c r="C1" s="234" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="254"/>
-      <c r="E1" s="254"/>
-      <c r="F1" s="254"/>
-      <c r="G1" s="254"/>
-      <c r="H1" s="254"/>
-      <c r="I1" s="254"/>
-      <c r="J1" s="254"/>
-      <c r="K1" s="254"/>
-      <c r="L1" s="254"/>
-      <c r="M1" s="254"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="235"/>
+      <c r="K1" s="235"/>
+      <c r="L1" s="235"/>
+      <c r="M1" s="235"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="245"/>
+      <c r="B2" s="226"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -11644,17 +11653,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="246" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="247"/>
+      <c r="B3" s="227" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="228"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="248" t="s">
+      <c r="H3" s="229" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="248"/>
+      <c r="I3" s="229"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -11670,14 +11679,14 @@
       <c r="D4" s="16">
         <v>44472</v>
       </c>
-      <c r="E4" s="249" t="s">
+      <c r="E4" s="230" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="250"/>
-      <c r="H4" s="251" t="s">
+      <c r="F4" s="231"/>
+      <c r="H4" s="232" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="252"/>
+      <c r="I4" s="233"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -11687,10 +11696,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="238" t="s">
+      <c r="P4" s="219" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="239"/>
+      <c r="Q4" s="220"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -12077,7 +12086,9 @@
       <c r="F13" s="25">
         <v>48834</v>
       </c>
-      <c r="G13" s="26"/>
+      <c r="G13" s="26" t="s">
+        <v>4</v>
+      </c>
       <c r="H13" s="32">
         <v>44481</v>
       </c>
@@ -12243,7 +12254,7 @@
         <v>6242</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E17" s="24">
         <v>44485</v>
@@ -12262,7 +12273,7 @@
         <v>44485</v>
       </c>
       <c r="K17" s="40" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="L17" s="43">
         <v>12019</v>
@@ -12290,36 +12301,41 @@
         <v>44486</v>
       </c>
       <c r="C18" s="22">
-        <v>0</v>
-      </c>
-      <c r="D18" s="31"/>
+        <v>214</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>195</v>
+      </c>
       <c r="E18" s="24">
         <v>44486</v>
       </c>
-      <c r="F18" s="25"/>
+      <c r="F18" s="25">
+        <v>89324</v>
+      </c>
       <c r="G18" s="26"/>
       <c r="H18" s="32">
         <v>44486</v>
       </c>
       <c r="I18" s="28">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="J18" s="33"/>
       <c r="K18" s="47"/>
       <c r="L18" s="35"/>
       <c r="M18" s="138">
-        <v>0</v>
+        <f>19690+65000</f>
+        <v>84690</v>
       </c>
       <c r="N18" s="30">
-        <v>0</v>
+        <v>4413</v>
       </c>
       <c r="P18" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>89324.5</v>
       </c>
       <c r="Q18" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R18" s="26"/>
     </row>
@@ -12335,26 +12351,29 @@
       <c r="E19" s="24">
         <v>44487</v>
       </c>
-      <c r="F19" s="25"/>
+      <c r="F19" s="25">
+        <v>57179</v>
+      </c>
       <c r="G19" s="26"/>
       <c r="H19" s="32">
         <v>44487</v>
       </c>
       <c r="I19" s="28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J19" s="33"/>
       <c r="K19" s="48"/>
       <c r="L19" s="49"/>
       <c r="M19" s="138">
-        <v>0</v>
+        <f>22800+34369</f>
+        <v>57169</v>
       </c>
       <c r="N19" s="30">
         <v>0</v>
       </c>
       <c r="P19" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>57179</v>
       </c>
       <c r="Q19" s="9">
         <f t="shared" si="1"/>
@@ -12374,26 +12393,29 @@
       <c r="E20" s="24">
         <v>44488</v>
       </c>
-      <c r="F20" s="25"/>
+      <c r="F20" s="25">
+        <v>49927</v>
+      </c>
       <c r="G20" s="26"/>
       <c r="H20" s="32">
         <v>44488</v>
       </c>
       <c r="I20" s="28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J20" s="33"/>
       <c r="K20" s="50"/>
       <c r="L20" s="43"/>
       <c r="M20" s="138">
-        <v>0</v>
+        <f>15000+31972</f>
+        <v>46972</v>
       </c>
       <c r="N20" s="30">
-        <v>0</v>
+        <v>2945</v>
       </c>
       <c r="P20" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>49927</v>
       </c>
       <c r="Q20" s="9">
         <f t="shared" si="1"/>
@@ -12407,32 +12429,37 @@
         <v>44489</v>
       </c>
       <c r="C21" s="22">
-        <v>0</v>
-      </c>
-      <c r="D21" s="31"/>
+        <v>5743</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>196</v>
+      </c>
       <c r="E21" s="24">
         <v>44489</v>
       </c>
-      <c r="F21" s="25"/>
+      <c r="F21" s="25">
+        <v>33425</v>
+      </c>
       <c r="G21" s="26"/>
       <c r="H21" s="32">
         <v>44489</v>
       </c>
       <c r="I21" s="28">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J21" s="33"/>
       <c r="K21" s="178"/>
       <c r="L21" s="43"/>
       <c r="M21" s="138">
-        <v>0</v>
+        <f>10000+17627</f>
+        <v>27627</v>
       </c>
       <c r="N21" s="30">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="P21" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>33425</v>
       </c>
       <c r="Q21" s="9">
         <f t="shared" si="1"/>
@@ -12452,30 +12479,32 @@
       <c r="E22" s="24">
         <v>44490</v>
       </c>
-      <c r="F22" s="25"/>
+      <c r="F22" s="25">
+        <v>35561</v>
+      </c>
       <c r="G22" s="26"/>
       <c r="H22" s="32">
         <v>44490</v>
       </c>
       <c r="I22" s="28">
-        <v>0</v>
+        <v>885</v>
       </c>
       <c r="J22" s="33"/>
       <c r="K22" s="51"/>
       <c r="L22" s="52"/>
       <c r="M22" s="138">
-        <v>0</v>
+        <f>10000+23676</f>
+        <v>33676</v>
       </c>
       <c r="N22" s="30">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="P22" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>35561</v>
+      </c>
+      <c r="Q22" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="R22" s="26"/>
     </row>
@@ -12485,32 +12514,37 @@
         <v>44491</v>
       </c>
       <c r="C23" s="22">
-        <v>0</v>
-      </c>
-      <c r="D23" s="31"/>
+        <v>1612</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>199</v>
+      </c>
       <c r="E23" s="24">
         <v>44491</v>
       </c>
-      <c r="F23" s="25"/>
+      <c r="F23" s="25">
+        <v>97455</v>
+      </c>
       <c r="G23" s="26"/>
       <c r="H23" s="32">
         <v>44491</v>
       </c>
       <c r="I23" s="28">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J23" s="53"/>
       <c r="K23" s="54"/>
       <c r="L23" s="43"/>
       <c r="M23" s="138">
-        <v>0</v>
+        <f>30000+45000+18535</f>
+        <v>93535</v>
       </c>
       <c r="N23" s="30">
-        <v>0</v>
+        <v>2288</v>
       </c>
       <c r="P23" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>97455</v>
       </c>
       <c r="Q23" s="9">
         <f t="shared" si="1"/>
@@ -13069,21 +13103,21 @@
       <c r="J39" s="67"/>
       <c r="K39" s="82"/>
       <c r="L39" s="69"/>
-      <c r="M39" s="240">
+      <c r="M39" s="221">
         <f>SUM(M5:M38)</f>
-        <v>675038</v>
-      </c>
-      <c r="N39" s="242">
+        <v>1018707</v>
+      </c>
+      <c r="N39" s="223">
         <f>SUM(N5:N38)</f>
-        <v>22988</v>
+        <v>33674</v>
       </c>
       <c r="P39" s="83">
         <f>SUM(P5:P38)</f>
-        <v>740792</v>
+        <v>1103663.5</v>
       </c>
       <c r="Q39" s="9">
         <f>SUM(Q5:Q38)</f>
-        <v>5720</v>
+        <v>5720.5</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -13099,8 +13133,8 @@
       <c r="J40" s="67"/>
       <c r="K40" s="71"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="241"/>
-      <c r="N40" s="243"/>
+      <c r="M40" s="222"/>
+      <c r="N40" s="224"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -13273,7 +13307,7 @@
       </c>
       <c r="C50" s="93">
         <f>SUM(C5:C49)</f>
-        <v>14361</v>
+        <v>21930</v>
       </c>
       <c r="D50" s="94"/>
       <c r="E50" s="95" t="s">
@@ -13281,7 +13315,7 @@
       </c>
       <c r="F50" s="96">
         <f>SUM(F5:F49)</f>
-        <v>735072</v>
+        <v>1097943</v>
       </c>
       <c r="G50" s="94"/>
       <c r="H50" s="97" t="s">
@@ -13289,7 +13323,7 @@
       </c>
       <c r="I50" s="98">
         <f>SUM(I5:I49)</f>
-        <v>172</v>
+        <v>1119.5</v>
       </c>
       <c r="J50" s="99"/>
       <c r="K50" s="100" t="s">
@@ -13315,32 +13349,32 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="228" t="s">
+      <c r="H52" s="245" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="229"/>
+      <c r="I52" s="246"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="230">
+      <c r="K52" s="247">
         <f>I50+L50</f>
-        <v>28405</v>
-      </c>
-      <c r="L52" s="231"/>
-      <c r="M52" s="219">
+        <v>29352.5</v>
+      </c>
+      <c r="L52" s="248"/>
+      <c r="M52" s="236">
         <f>N39+M39</f>
-        <v>698026</v>
-      </c>
-      <c r="N52" s="220"/>
+        <v>1052381</v>
+      </c>
+      <c r="N52" s="237"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="232" t="s">
+      <c r="D53" s="249" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="232"/>
+      <c r="E53" s="249"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
-        <v>692306</v>
+        <v>1046660.5</v>
       </c>
       <c r="I53" s="108"/>
       <c r="J53" s="109"/>
@@ -13348,22 +13382,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="233" t="s">
+      <c r="D54" s="250" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="233"/>
+      <c r="E54" s="250"/>
       <c r="F54" s="102">
         <v>0</v>
       </c>
-      <c r="I54" s="234" t="s">
+      <c r="I54" s="251" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="235"/>
-      <c r="K54" s="236">
+      <c r="J54" s="252"/>
+      <c r="K54" s="253">
         <f>F56+F57+F58</f>
-        <v>692306</v>
-      </c>
-      <c r="L54" s="237"/>
+        <v>1046660.5</v>
+      </c>
+      <c r="L54" s="254"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -13387,18 +13421,18 @@
       </c>
       <c r="F56" s="102">
         <f>SUM(F53:F55)</f>
-        <v>692306</v>
+        <v>1046660.5</v>
       </c>
       <c r="H56" s="20"/>
       <c r="I56" s="116" t="s">
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="221">
+      <c r="K56" s="238">
         <f>-C4</f>
         <v>-134848.89000000001</v>
       </c>
-      <c r="L56" s="222"/>
+      <c r="L56" s="239"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -13415,22 +13449,22 @@
       <c r="C58" s="120">
         <v>44472</v>
       </c>
-      <c r="D58" s="223" t="s">
+      <c r="D58" s="240" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="224"/>
+      <c r="E58" s="241"/>
       <c r="F58" s="121">
         <v>0</v>
       </c>
-      <c r="I58" s="225" t="s">
+      <c r="I58" s="242" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="226"/>
-      <c r="K58" s="227">
+      <c r="J58" s="243"/>
+      <c r="K58" s="244">
         <f>K54+K56</f>
-        <v>557457.11</v>
-      </c>
-      <c r="L58" s="227"/>
+        <v>911811.61</v>
+      </c>
+      <c r="L58" s="244"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -13574,12 +13608,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -13594,6 +13622,12 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.17" right="0.16" top="0.3" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14939,7 +14973,7 @@
   <dimension ref="A23:G54"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14971,22 +15005,22 @@
     </row>
     <row r="46" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="169">
-        <v>44485</v>
+        <v>44490</v>
       </c>
       <c r="B46" s="170" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C46" s="171">
-        <v>654.9</v>
+        <v>1684.95</v>
       </c>
       <c r="D46" s="172" t="s">
         <v>32</v>
       </c>
       <c r="E46" s="173" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="F46" s="107">
-        <v>249</v>
+        <v>485</v>
       </c>
       <c r="G46" s="210"/>
     </row>

</xml_diff>